<commit_message>
Got movement working. I can now move an arbitrary piece to an arbitrary location. I need to add move logic, ie: piece move sets, is a piece in the selected spot, is the move path clear, etc.
</commit_message>
<xml_diff>
--- a/Gambit/Chess.xlsx
+++ b/Gambit/Chess.xlsx
@@ -117,10 +117,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -429,12 +429,12 @@
   <dimension ref="A2:CF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:S11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="5" customWidth="1"/>
     <col min="2" max="10" width="2.7109375" customWidth="1"/>
     <col min="20" max="20" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="84" width="9.140625" style="2" customWidth="1"/>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="11" spans="1:84" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="5"/>
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1746,17 +1746,17 @@
       <c r="J11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="5" t="str">
+      <c r="L11" s="6" t="str">
         <f>(L10&amp;L9&amp;L8&amp;L7&amp;L6&amp;L5&amp;L4&amp;L3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
       <c r="T11" s="3">
         <f>SUM(T2:T10)</f>
         <v>0</v>
@@ -1827,16 +1827,16 @@
       <c r="CF11" s="3"/>
     </row>
     <row r="12" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Fixed the excel sheet.
</commit_message>
<xml_diff>
--- a/Gambit/Chess.xlsx
+++ b/Gambit/Chess.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -104,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -125,11 +125,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -426,220 +472,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CF12"/>
+  <dimension ref="A1:CQ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="5" customWidth="1"/>
-    <col min="2" max="10" width="2.7109375" customWidth="1"/>
-    <col min="20" max="20" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="84" width="9.140625" style="2" customWidth="1"/>
+    <col min="1" max="10" width="2.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="13" max="21" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="21.42578125" customWidth="1"/>
+    <col min="32" max="95" width="9.140625" style="2" customWidth="1"/>
+    <col min="96" max="96" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="T2" s="2">
-        <f>SUM(U5:AB5)</f>
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
+    <row r="1" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+    </row>
+    <row r="2" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="AE2" s="2">
+        <f>SUM(AF5:AM5)</f>
+        <v>8</v>
+      </c>
+      <c r="AF2" s="2">
         <v>1</v>
       </c>
-      <c r="V2" s="2">
+      <c r="AG2" s="2">
         <v>2</v>
       </c>
-      <c r="W2" s="2">
+      <c r="AH2" s="2">
         <v>3</v>
       </c>
-      <c r="X2" s="2">
+      <c r="AI2" s="2">
         <v>4</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="AJ2" s="2">
         <v>5</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AK2" s="2">
         <v>6</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AL2" s="2">
         <v>7</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AM2" s="2">
         <v>8</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AN2" s="2">
         <v>9</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AO2" s="2">
         <v>10</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AP2" s="2">
         <v>11</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AQ2" s="2">
         <v>12</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AR2" s="2">
         <v>13</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AS2" s="2">
         <v>14</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AT2" s="2">
         <v>15</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="AU2" s="2">
         <v>16</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="AV2" s="2">
         <v>17</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="AW2" s="2">
         <v>18</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AX2" s="2">
         <v>19</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AY2" s="2">
         <v>20</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AZ2" s="2">
         <v>21</v>
       </c>
-      <c r="AP2" s="2">
+      <c r="BA2" s="2">
         <v>22</v>
       </c>
-      <c r="AQ2" s="2">
+      <c r="BB2" s="2">
         <v>23</v>
       </c>
-      <c r="AR2" s="2">
+      <c r="BC2" s="2">
         <v>24</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="BD2" s="2">
         <v>25</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="BE2" s="2">
         <v>26</v>
       </c>
-      <c r="AU2" s="2">
+      <c r="BF2" s="2">
         <v>27</v>
       </c>
-      <c r="AV2" s="2">
+      <c r="BG2" s="2">
         <v>28</v>
       </c>
-      <c r="AW2" s="2">
+      <c r="BH2" s="2">
         <v>29</v>
       </c>
-      <c r="AX2" s="2">
+      <c r="BI2" s="2">
         <v>30</v>
       </c>
-      <c r="AY2" s="2">
+      <c r="BJ2" s="2">
         <v>31</v>
       </c>
-      <c r="AZ2" s="2">
+      <c r="BK2" s="2">
         <v>32</v>
       </c>
-      <c r="BA2" s="2">
+      <c r="BL2" s="2">
         <v>33</v>
       </c>
-      <c r="BB2" s="2">
+      <c r="BM2" s="2">
         <v>34</v>
       </c>
-      <c r="BC2" s="2">
+      <c r="BN2" s="2">
         <v>35</v>
       </c>
-      <c r="BD2" s="2">
+      <c r="BO2" s="2">
         <v>36</v>
       </c>
-      <c r="BE2" s="2">
+      <c r="BP2" s="2">
         <v>37</v>
       </c>
-      <c r="BF2" s="2">
+      <c r="BQ2" s="2">
         <v>38</v>
       </c>
-      <c r="BG2" s="2">
+      <c r="BR2" s="2">
         <v>39</v>
       </c>
-      <c r="BH2" s="2">
+      <c r="BS2" s="2">
         <v>40</v>
       </c>
-      <c r="BI2" s="2">
+      <c r="BT2" s="2">
         <v>41</v>
       </c>
-      <c r="BJ2" s="2">
+      <c r="BU2" s="2">
         <v>42</v>
       </c>
-      <c r="BK2" s="2">
+      <c r="BV2" s="2">
         <v>43</v>
       </c>
-      <c r="BL2" s="2">
+      <c r="BW2" s="2">
         <v>44</v>
       </c>
-      <c r="BM2" s="2">
+      <c r="BX2" s="2">
         <v>45</v>
       </c>
-      <c r="BN2" s="2">
+      <c r="BY2" s="2">
         <v>46</v>
       </c>
-      <c r="BO2" s="2">
+      <c r="BZ2" s="2">
         <v>47</v>
       </c>
-      <c r="BP2" s="2">
+      <c r="CA2" s="2">
         <v>48</v>
       </c>
-      <c r="BQ2" s="2">
+      <c r="CB2" s="2">
         <v>49</v>
       </c>
-      <c r="BR2" s="2">
+      <c r="CC2" s="2">
         <v>50</v>
       </c>
-      <c r="BS2" s="2">
+      <c r="CD2" s="2">
         <v>51</v>
       </c>
-      <c r="BT2" s="2">
+      <c r="CE2" s="2">
         <v>52</v>
       </c>
-      <c r="BU2" s="2">
+      <c r="CF2" s="2">
         <v>53</v>
       </c>
-      <c r="BV2" s="2">
+      <c r="CG2" s="2">
         <v>54</v>
       </c>
-      <c r="BW2" s="2">
+      <c r="CH2" s="2">
         <v>55</v>
       </c>
-      <c r="BX2" s="2">
+      <c r="CI2" s="2">
         <v>56</v>
       </c>
-      <c r="BY2" s="2">
+      <c r="CJ2" s="2">
         <v>57</v>
       </c>
-      <c r="BZ2" s="2">
+      <c r="CK2" s="2">
         <v>58</v>
       </c>
-      <c r="CA2" s="2">
+      <c r="CL2" s="2">
         <v>59</v>
       </c>
-      <c r="CB2" s="2">
+      <c r="CM2" s="2">
         <v>60</v>
       </c>
-      <c r="CC2" s="2">
+      <c r="CN2" s="2">
         <v>61</v>
       </c>
-      <c r="CD2" s="2">
+      <c r="CO2" s="2">
         <v>62</v>
       </c>
-      <c r="CE2" s="2">
+      <c r="CP2" s="2">
         <v>63</v>
       </c>
-      <c r="CF2" s="2">
+      <c r="CQ2" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:95" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -669,274 +723,312 @@
       <c r="J3" s="4">
         <v>0</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L9" si="0">(C3&amp;D3&amp;E3&amp;F3&amp;G3&amp;H3&amp;I3&amp;J3)</f>
+      <c r="L3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3" s="4">
+        <f>J10</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <f>I10</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
+        <f>G10</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <f>F10</f>
+        <v>1</v>
+      </c>
+      <c r="S3" s="4">
+        <f>E10</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="4">
+        <f>D10</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="4">
+        <f>C10</f>
+        <v>0</v>
+      </c>
+      <c r="W3" t="str">
+        <f t="shared" ref="W3:W9" si="0">(J3&amp;I3&amp;H3&amp;G3&amp;F3&amp;E3&amp;D3&amp;C3)</f>
         <v>00000000</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="T3" s="2">
-        <f>SUM(AC5:AJ5)</f>
-        <v>0</v>
-      </c>
-      <c r="U3" s="2">
-        <f>(U2^2)</f>
+      <c r="X3" s="1"/>
+      <c r="AE3" s="2">
+        <f>SUM(AN5:AU5)</f>
+        <v>0</v>
+      </c>
+      <c r="AF3" s="2">
+        <f>(AF2^2)</f>
         <v>1</v>
       </c>
-      <c r="V3" s="2">
-        <f>U3*2</f>
+      <c r="AG3" s="2">
+        <f>AF3*2</f>
         <v>2</v>
       </c>
-      <c r="W3" s="2">
-        <f t="shared" ref="W3:CF3" si="1">V3*2</f>
+      <c r="AH3" s="2">
+        <f t="shared" ref="AH3:CQ3" si="1">AG3*2</f>
         <v>4</v>
       </c>
-      <c r="X3" s="2">
+      <c r="AI3" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="AJ3" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AK3" s="2">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AL3" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AM3" s="2">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AN3" s="2">
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AO3" s="2">
         <f t="shared" si="1"/>
         <v>512</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AP3" s="2">
         <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AQ3" s="2">
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AR3" s="2">
         <f t="shared" si="1"/>
         <v>4096</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="AS3" s="2">
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AT3" s="2">
         <f t="shared" si="1"/>
         <v>16384</v>
       </c>
-      <c r="AJ3" s="2">
+      <c r="AU3" s="2">
         <f t="shared" si="1"/>
         <v>32768</v>
       </c>
-      <c r="AK3" s="2">
+      <c r="AV3" s="2">
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-      <c r="AL3" s="2">
+      <c r="AW3" s="2">
         <f t="shared" si="1"/>
         <v>131072</v>
       </c>
-      <c r="AM3" s="2">
+      <c r="AX3" s="2">
         <f t="shared" si="1"/>
         <v>262144</v>
       </c>
-      <c r="AN3" s="2">
+      <c r="AY3" s="2">
         <f t="shared" si="1"/>
         <v>524288</v>
       </c>
-      <c r="AO3" s="2">
+      <c r="AZ3" s="2">
         <f t="shared" si="1"/>
         <v>1048576</v>
       </c>
-      <c r="AP3" s="2">
+      <c r="BA3" s="2">
         <f t="shared" si="1"/>
         <v>2097152</v>
       </c>
-      <c r="AQ3" s="2">
+      <c r="BB3" s="2">
         <f t="shared" si="1"/>
         <v>4194304</v>
       </c>
-      <c r="AR3" s="2">
+      <c r="BC3" s="2">
         <f t="shared" si="1"/>
         <v>8388608</v>
       </c>
-      <c r="AS3" s="2">
+      <c r="BD3" s="2">
         <f t="shared" si="1"/>
         <v>16777216</v>
       </c>
-      <c r="AT3" s="2">
+      <c r="BE3" s="2">
         <f t="shared" si="1"/>
         <v>33554432</v>
       </c>
-      <c r="AU3" s="2">
+      <c r="BF3" s="2">
         <f t="shared" si="1"/>
         <v>67108864</v>
       </c>
-      <c r="AV3" s="2">
+      <c r="BG3" s="2">
         <f t="shared" si="1"/>
         <v>134217728</v>
       </c>
-      <c r="AW3" s="2">
+      <c r="BH3" s="2">
         <f t="shared" si="1"/>
         <v>268435456</v>
       </c>
-      <c r="AX3" s="2">
+      <c r="BI3" s="2">
         <f t="shared" si="1"/>
         <v>536870912</v>
       </c>
-      <c r="AY3" s="2">
+      <c r="BJ3" s="2">
         <f t="shared" si="1"/>
         <v>1073741824</v>
       </c>
-      <c r="AZ3" s="2">
+      <c r="BK3" s="2">
         <f t="shared" si="1"/>
         <v>2147483648</v>
       </c>
-      <c r="BA3" s="2">
+      <c r="BL3" s="2">
         <f t="shared" si="1"/>
         <v>4294967296</v>
       </c>
-      <c r="BB3" s="2">
+      <c r="BM3" s="2">
         <f t="shared" si="1"/>
         <v>8589934592</v>
       </c>
-      <c r="BC3" s="2">
+      <c r="BN3" s="2">
         <f t="shared" si="1"/>
         <v>17179869184</v>
       </c>
-      <c r="BD3" s="2">
+      <c r="BO3" s="2">
         <f t="shared" si="1"/>
         <v>34359738368</v>
       </c>
-      <c r="BE3" s="2">
+      <c r="BP3" s="2">
         <f t="shared" si="1"/>
         <v>68719476736</v>
       </c>
-      <c r="BF3" s="2">
+      <c r="BQ3" s="2">
         <f t="shared" si="1"/>
         <v>137438953472</v>
       </c>
-      <c r="BG3" s="2">
+      <c r="BR3" s="2">
         <f t="shared" si="1"/>
         <v>274877906944</v>
       </c>
-      <c r="BH3" s="2">
+      <c r="BS3" s="2">
         <f t="shared" si="1"/>
         <v>549755813888</v>
       </c>
-      <c r="BI3" s="2">
+      <c r="BT3" s="2">
         <f t="shared" si="1"/>
         <v>1099511627776</v>
       </c>
-      <c r="BJ3" s="2">
+      <c r="BU3" s="2">
         <f t="shared" si="1"/>
         <v>2199023255552</v>
       </c>
-      <c r="BK3" s="2">
+      <c r="BV3" s="2">
         <f t="shared" si="1"/>
         <v>4398046511104</v>
       </c>
-      <c r="BL3" s="2">
+      <c r="BW3" s="2">
         <f t="shared" si="1"/>
         <v>8796093022208</v>
       </c>
-      <c r="BM3" s="2">
+      <c r="BX3" s="2">
         <f t="shared" si="1"/>
         <v>17592186044416</v>
       </c>
-      <c r="BN3" s="2">
+      <c r="BY3" s="2">
         <f t="shared" si="1"/>
         <v>35184372088832</v>
       </c>
-      <c r="BO3" s="2">
+      <c r="BZ3" s="2">
         <f t="shared" si="1"/>
         <v>70368744177664</v>
       </c>
-      <c r="BP3" s="2">
+      <c r="CA3" s="2">
         <f t="shared" si="1"/>
         <v>140737488355328</v>
       </c>
-      <c r="BQ3" s="2">
+      <c r="CB3" s="2">
         <f t="shared" si="1"/>
         <v>281474976710656</v>
       </c>
-      <c r="BR3" s="2">
+      <c r="CC3" s="2">
         <f t="shared" si="1"/>
         <v>562949953421312</v>
       </c>
-      <c r="BS3" s="2">
+      <c r="CD3" s="2">
         <f t="shared" si="1"/>
         <v>1125899906842624</v>
       </c>
-      <c r="BT3" s="2">
+      <c r="CE3" s="2">
         <f t="shared" si="1"/>
         <v>2251799813685248</v>
       </c>
-      <c r="BU3" s="2">
+      <c r="CF3" s="2">
         <f t="shared" si="1"/>
         <v>4503599627370496</v>
       </c>
-      <c r="BV3" s="2">
+      <c r="CG3" s="2">
         <f t="shared" si="1"/>
         <v>9007199254740992</v>
       </c>
-      <c r="BW3" s="2">
+      <c r="CH3" s="2">
         <f t="shared" si="1"/>
         <v>1.8014398509481984E+16</v>
       </c>
-      <c r="BX3" s="2">
+      <c r="CI3" s="2">
         <f t="shared" si="1"/>
         <v>3.6028797018963968E+16</v>
       </c>
-      <c r="BY3" s="2">
+      <c r="CJ3" s="2">
         <f t="shared" si="1"/>
         <v>7.2057594037927936E+16</v>
       </c>
-      <c r="BZ3" s="2">
+      <c r="CK3" s="2">
         <f t="shared" si="1"/>
         <v>1.4411518807585587E+17</v>
       </c>
-      <c r="CA3" s="2">
+      <c r="CL3" s="2">
         <f t="shared" si="1"/>
         <v>2.8823037615171174E+17</v>
       </c>
-      <c r="CB3" s="2">
+      <c r="CM3" s="2">
         <f t="shared" si="1"/>
         <v>5.7646075230342349E+17</v>
       </c>
-      <c r="CC3" s="2">
+      <c r="CN3" s="2">
         <f t="shared" si="1"/>
         <v>1.152921504606847E+18</v>
       </c>
-      <c r="CD3" s="2">
+      <c r="CO3" s="2">
         <f t="shared" si="1"/>
         <v>2.305843009213694E+18</v>
       </c>
-      <c r="CE3" s="2">
+      <c r="CP3" s="2">
         <f t="shared" si="1"/>
         <v>4.6116860184273879E+18</v>
       </c>
-      <c r="CF3" s="2">
+      <c r="CQ3" s="2">
         <f t="shared" si="1"/>
         <v>9.2233720368547758E+18</v>
       </c>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4">
         <v>7</v>
       </c>
@@ -964,274 +1056,310 @@
       <c r="J4" s="4">
         <v>0</v>
       </c>
-      <c r="L4" t="str">
+      <c r="L4" s="9"/>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4" s="4">
+        <f>J9</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <f>I9</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <f>H9</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>G9</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <f>F9</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <f>E9</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <f>D9</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <f>C9</f>
+        <v>0</v>
+      </c>
+      <c r="W4" t="str">
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="T4" s="2">
-        <f>SUM(AK5:AR5)</f>
-        <v>0</v>
-      </c>
-      <c r="U4" s="2">
-        <f>J3</f>
-        <v>0</v>
-      </c>
-      <c r="V4" s="2">
-        <f>I3</f>
-        <v>0</v>
-      </c>
-      <c r="W4" s="2">
-        <f>H3</f>
-        <v>0</v>
-      </c>
-      <c r="X4" s="2">
-        <f>G3</f>
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2">
-        <f>F3</f>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="2">
-        <f>E3</f>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="2">
-        <f>D3</f>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="2">
-        <f>C3</f>
-        <v>0</v>
-      </c>
-      <c r="AC4" s="2">
-        <f>J4</f>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="2">
-        <f>I4</f>
-        <v>0</v>
-      </c>
+      <c r="X4" s="1"/>
       <c r="AE4" s="2">
-        <f>H4</f>
+        <f>SUM(AV5:BC5)</f>
         <v>0</v>
       </c>
       <c r="AF4" s="2">
-        <f>G4</f>
+        <f>$C10</f>
         <v>0</v>
       </c>
       <c r="AG4" s="2">
-        <f>F4</f>
+        <f>$D10</f>
         <v>0</v>
       </c>
       <c r="AH4" s="2">
-        <f>E4</f>
+        <f>$E10</f>
         <v>0</v>
       </c>
       <c r="AI4" s="2">
-        <f>D4</f>
-        <v>0</v>
+        <f>$F10</f>
+        <v>1</v>
       </c>
       <c r="AJ4" s="2">
-        <f>C4</f>
+        <f>$G10</f>
         <v>0</v>
       </c>
       <c r="AK4" s="2">
-        <f>J5</f>
+        <f>$H10</f>
         <v>0</v>
       </c>
       <c r="AL4" s="2">
-        <f>I5</f>
+        <f>$I10</f>
         <v>0</v>
       </c>
       <c r="AM4" s="2">
-        <f>H5</f>
+        <f>$J10</f>
         <v>0</v>
       </c>
       <c r="AN4" s="2">
-        <f>G5</f>
+        <f>$C9</f>
         <v>0</v>
       </c>
       <c r="AO4" s="2">
-        <f>F5</f>
+        <f>$D9</f>
         <v>0</v>
       </c>
       <c r="AP4" s="2">
-        <f>E5</f>
+        <f>$E9</f>
         <v>0</v>
       </c>
       <c r="AQ4" s="2">
-        <f>D5</f>
+        <f>$F9</f>
         <v>0</v>
       </c>
       <c r="AR4" s="2">
-        <f>C5</f>
+        <f>$G9</f>
         <v>0</v>
       </c>
       <c r="AS4" s="2">
-        <f>J6</f>
+        <f>$H9</f>
         <v>0</v>
       </c>
       <c r="AT4" s="2">
-        <f>I6</f>
+        <f>$I9</f>
         <v>0</v>
       </c>
       <c r="AU4" s="2">
-        <f>H6</f>
+        <f>$J9</f>
         <v>0</v>
       </c>
       <c r="AV4" s="2">
-        <f>G6</f>
+        <f>J8</f>
         <v>0</v>
       </c>
       <c r="AW4" s="2">
-        <f>F6</f>
+        <f>I8</f>
         <v>0</v>
       </c>
       <c r="AX4" s="2">
-        <f>E6</f>
+        <f>H8</f>
         <v>0</v>
       </c>
       <c r="AY4" s="2">
-        <f>D6</f>
+        <f>G8</f>
         <v>0</v>
       </c>
       <c r="AZ4" s="2">
-        <f>C6</f>
+        <f>F8</f>
         <v>0</v>
       </c>
       <c r="BA4" s="2">
-        <f>J7</f>
+        <f>E8</f>
         <v>0</v>
       </c>
       <c r="BB4" s="2">
-        <f>I7</f>
+        <f>D8</f>
         <v>0</v>
       </c>
       <c r="BC4" s="2">
-        <f>H7</f>
+        <f>J8</f>
         <v>0</v>
       </c>
       <c r="BD4" s="2">
-        <f>G7</f>
+        <f>$C7</f>
         <v>0</v>
       </c>
       <c r="BE4" s="2">
-        <f>F7</f>
+        <f>$D7</f>
         <v>0</v>
       </c>
       <c r="BF4" s="2">
-        <f>E7</f>
+        <f>$E7</f>
         <v>0</v>
       </c>
       <c r="BG4" s="2">
-        <f>D7</f>
+        <f>$F7</f>
         <v>0</v>
       </c>
       <c r="BH4" s="2">
-        <f>C7</f>
+        <f>$G7</f>
         <v>0</v>
       </c>
       <c r="BI4" s="2">
-        <f>J8</f>
+        <f>$H7</f>
         <v>0</v>
       </c>
       <c r="BJ4" s="2">
-        <f>I8</f>
+        <f>$I7</f>
         <v>0</v>
       </c>
       <c r="BK4" s="2">
-        <f>H8</f>
+        <f>$J7</f>
         <v>0</v>
       </c>
       <c r="BL4" s="2">
-        <f>G8</f>
+        <f>$C6</f>
         <v>0</v>
       </c>
       <c r="BM4" s="2">
-        <f>F8</f>
+        <f>$D6</f>
         <v>0</v>
       </c>
       <c r="BN4" s="2">
-        <f>E8</f>
+        <f>$E6</f>
         <v>0</v>
       </c>
       <c r="BO4" s="2">
-        <f>D8</f>
+        <f>$F6</f>
         <v>0</v>
       </c>
       <c r="BP4" s="2">
-        <f>C8</f>
+        <f>$G6</f>
         <v>0</v>
       </c>
       <c r="BQ4" s="2">
-        <f>J9</f>
+        <f>$H6</f>
         <v>0</v>
       </c>
       <c r="BR4" s="2">
-        <f>I9</f>
+        <f>$I6</f>
         <v>0</v>
       </c>
       <c r="BS4" s="2">
-        <f>H9</f>
+        <f>$J6</f>
         <v>0</v>
       </c>
       <c r="BT4" s="2">
-        <f>G9</f>
+        <f>$C5</f>
         <v>0</v>
       </c>
       <c r="BU4" s="2">
-        <f>F9</f>
+        <f>$D5</f>
         <v>0</v>
       </c>
       <c r="BV4" s="2">
-        <f>E9</f>
+        <f>$E5</f>
         <v>0</v>
       </c>
       <c r="BW4" s="2">
-        <f>D9</f>
+        <f>$F5</f>
         <v>0</v>
       </c>
       <c r="BX4" s="2">
-        <f>C9</f>
+        <f>$G5</f>
         <v>0</v>
       </c>
       <c r="BY4" s="2">
-        <f>J10</f>
+        <f>$H5</f>
         <v>0</v>
       </c>
       <c r="BZ4" s="2">
-        <f>I10</f>
+        <f>$I5</f>
         <v>0</v>
       </c>
       <c r="CA4" s="2">
-        <f>H10</f>
+        <f>$J5</f>
         <v>0</v>
       </c>
       <c r="CB4" s="2">
-        <f>G10</f>
+        <f>$C4</f>
         <v>0</v>
       </c>
       <c r="CC4" s="2">
-        <f>F10</f>
+        <f>$D4</f>
         <v>0</v>
       </c>
       <c r="CD4" s="2">
-        <f>E10</f>
+        <f>$E4</f>
         <v>0</v>
       </c>
       <c r="CE4" s="2">
-        <f>D10</f>
+        <f>$F4</f>
         <v>0</v>
       </c>
       <c r="CF4" s="2">
-        <f>C10</f>
+        <f>$G4</f>
+        <v>0</v>
+      </c>
+      <c r="CG4" s="2">
+        <f>$H4</f>
+        <v>0</v>
+      </c>
+      <c r="CH4" s="2">
+        <f>$I4</f>
+        <v>0</v>
+      </c>
+      <c r="CI4" s="2">
+        <f>$J4</f>
+        <v>0</v>
+      </c>
+      <c r="CJ4" s="2">
+        <f>$C3</f>
+        <v>0</v>
+      </c>
+      <c r="CK4" s="2">
+        <f>$D3</f>
+        <v>0</v>
+      </c>
+      <c r="CL4" s="2">
+        <f>$E3</f>
+        <v>0</v>
+      </c>
+      <c r="CM4" s="2">
+        <f>$F3</f>
+        <v>0</v>
+      </c>
+      <c r="CN4" s="2">
+        <f>$G3</f>
+        <v>0</v>
+      </c>
+      <c r="CO4" s="2">
+        <f>$H3</f>
+        <v>0</v>
+      </c>
+      <c r="CP4" s="2">
+        <f>$I3</f>
+        <v>0</v>
+      </c>
+      <c r="CQ4" s="2">
+        <f>$J3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5">
         <v>6</v>
       </c>
@@ -1259,65 +1387,57 @@
       <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="L5" t="str">
+      <c r="L5" s="9"/>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5" s="4">
+        <f>J8</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <f>I8</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <f>H8</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <f>G8</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="4">
+        <f>F8</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <f>E8</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="4">
+        <f>D8</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="4">
+        <f>C8</f>
+        <v>0</v>
+      </c>
+      <c r="W5" t="str">
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="T5" s="2">
-        <f>SUM(AS5:AZ5)</f>
-        <v>0</v>
-      </c>
-      <c r="U5" s="2">
-        <f t="shared" ref="U5:CE5" si="2">IF(U4=1,U3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="W5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="X5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AD5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="X5" s="1"/>
       <c r="AE5" s="2">
-        <f t="shared" si="2"/>
+        <f>SUM(BD5:BK5)</f>
         <v>0</v>
       </c>
       <c r="AF5" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(AF4=1,AF3,0)</f>
         <v>0</v>
       </c>
       <c r="AG5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AF5:CP5" si="2">IF(AG4=1,AG3,0)</f>
         <v>0</v>
       </c>
       <c r="AH5" s="2">
@@ -1326,7 +1446,7 @@
       </c>
       <c r="AI5" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AJ5" s="2">
         <f t="shared" si="2"/>
@@ -1521,12 +1641,56 @@
         <v>0</v>
       </c>
       <c r="CF5" s="2">
-        <f t="shared" ref="CF5" si="3">IF(CF4=1,CF3,0)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CG5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CH5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CI5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CJ5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CK5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CL5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CM5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CN5" s="2">
+        <f>IF(CN4=1,CN3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CO5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CP5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="CQ5" s="2">
+        <f t="shared" ref="CQ5" si="3">IF(CQ4=1,CQ3,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+    <row r="6" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -1554,18 +1718,54 @@
       <c r="J6" s="4">
         <v>0</v>
       </c>
-      <c r="L6" t="str">
+      <c r="L6" s="9"/>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6" s="4">
+        <f>J7</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <f>I7</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <f>H7</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4">
+        <f>G7</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="4">
+        <f>F7</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="4">
+        <f>E7</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="4">
+        <f>D7</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="4">
+        <f>C7</f>
+        <v>0</v>
+      </c>
+      <c r="W6" t="str">
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="T6" s="2">
-        <f>SUM(AS5:AZ5)</f>
+      <c r="X6" s="1"/>
+      <c r="AE6" s="2">
+        <f>SUM(BD5:BK5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7">
         <v>4</v>
       </c>
@@ -1593,18 +1793,54 @@
       <c r="J7" s="4">
         <v>0</v>
       </c>
-      <c r="L7" t="str">
+      <c r="L7" s="9"/>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7" s="4">
+        <f>J6</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <f>I6</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <f>H6</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <f>G6</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <f>F6</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <f>E6</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="4">
+        <f>D6</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="4">
+        <f>C6</f>
+        <v>0</v>
+      </c>
+      <c r="W7" t="str">
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="T7" s="2">
-        <f>SUM(BA5:BH5)</f>
+      <c r="X7" s="1"/>
+      <c r="AE7" s="2">
+        <f>SUM(BL5:BS5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
       <c r="B8">
         <v>3</v>
       </c>
@@ -1632,18 +1868,54 @@
       <c r="J8" s="4">
         <v>0</v>
       </c>
-      <c r="L8" t="str">
+      <c r="L8" s="9"/>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8" s="4">
+        <f>J5</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <f>I5</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>G5</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <f>F5</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="4">
+        <f>E5</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="4">
+        <f>C5</f>
+        <v>0</v>
+      </c>
+      <c r="W8" t="str">
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="T8" s="2">
-        <f>SUM(BI5:BP5)</f>
+      <c r="X8" s="1"/>
+      <c r="AE8" s="2">
+        <f>SUM(BT5:CA5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
       <c r="B9">
         <v>2</v>
       </c>
@@ -1671,18 +1943,54 @@
       <c r="J9" s="4">
         <v>0</v>
       </c>
-      <c r="L9" t="str">
+      <c r="L9" s="9"/>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9" s="4">
+        <f>J4</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <f>I4</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <f>H4</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <f>G4</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <f>F4</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <f>E4</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <f>D4</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="4">
+        <f>C4</f>
+        <v>0</v>
+      </c>
+      <c r="W9" t="str">
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="T9" s="2">
-        <f>SUM(BQ5:BX5)</f>
+      <c r="X9" s="1"/>
+      <c r="AE9" s="2">
+        <f>SUM(CB5:CI5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
       <c r="B10">
         <v>1</v>
       </c>
@@ -1696,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -1710,68 +2018,120 @@
       <c r="J10" s="4">
         <v>0</v>
       </c>
-      <c r="L10" t="str">
-        <f>(C10&amp;D10&amp;E10&amp;F10&amp;G10&amp;H10&amp;I10&amp;J10)</f>
-        <v>00000000</v>
-      </c>
-      <c r="M10" s="1"/>
-      <c r="T10" s="2">
-        <f>SUM(BY5:CF5)</f>
+      <c r="L10" s="9"/>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
+        <f>J3</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <f>I3</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <f>H3</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <f>G3</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="4">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="4">
+        <f>E3</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="4">
+        <f>D3</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="4">
+        <f>C3</f>
+        <v>0</v>
+      </c>
+      <c r="W10" t="str">
+        <f>(J10&amp;I10&amp;H10&amp;G10&amp;F10&amp;E10&amp;D10&amp;C10)</f>
+        <v>00001000</v>
+      </c>
+      <c r="X10" s="1"/>
+      <c r="AE10" s="2">
+        <f>SUM(CJ5:CQ5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:84" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
+    <row r="11" spans="1:95" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="6" t="str">
-        <f>(L10&amp;L9&amp;L8&amp;L7&amp;L6&amp;L5&amp;L4&amp;L3)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000</v>
-      </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="3">
-        <f>SUM(T2:T10)</f>
-        <v>0</v>
-      </c>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W11" s="8" t="str">
+        <f>(W3&amp;W4&amp;W5&amp;W6&amp;W7&amp;W8&amp;W9&amp;W10)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000001000</v>
+      </c>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="3">
+        <f>SUM(AE2:AE10)</f>
+        <v>8</v>
+      </c>
       <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
@@ -1825,25 +2185,58 @@
       <c r="CD11" s="3"/>
       <c r="CE11" s="3"/>
       <c r="CF11" s="3"/>
+      <c r="CG11" s="3"/>
+      <c r="CH11" s="3"/>
+      <c r="CI11" s="3"/>
+      <c r="CJ11" s="3"/>
+      <c r="CK11" s="3"/>
+      <c r="CL11" s="3"/>
+      <c r="CM11" s="3"/>
+      <c r="CN11" s="3"/>
+      <c r="CO11" s="3"/>
+      <c r="CP11" s="3"/>
+      <c r="CQ11" s="3"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="C12" s="6" t="s">
+    <row r="12" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="L12" s="7"/>
+      <c r="N12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="L11:S11"/>
+  <mergeCells count="5">
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="C12:J12"/>
+    <mergeCell ref="W11:AD11"/>
+    <mergeCell ref="L3:L10"/>
+    <mergeCell ref="N12:U12"/>
   </mergeCells>
+  <conditionalFormatting sqref="N3:U10">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C3:J10">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>

</xml_diff>

<commit_message>
Got the board flipped around. The bitmasks for move-attacks works beautifully. Just need to implement it to auto generate for each piece when selecting it to move/attack and the add logic that uses the masks.
</commit_message>
<xml_diff>
--- a/Gambit/Chess.xlsx
+++ b/Gambit/Chess.xlsx
@@ -126,36 +126,16 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -475,7 +455,7 @@
   <dimension ref="A1:CQ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +477,7 @@
       <c r="L2" s="7"/>
       <c r="AE2" s="2">
         <f>SUM(AF5:AM5)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AF2" s="2">
         <v>1</v>
@@ -693,7 +673,7 @@
       </c>
     </row>
     <row r="3" spans="1:95" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -723,7 +703,7 @@
       <c r="J3" s="4">
         <v>0</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="M3">
@@ -747,7 +727,7 @@
       </c>
       <c r="R3" s="4">
         <f>F10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="4">
         <f>E10</f>
@@ -1028,7 +1008,7 @@
       </c>
     </row>
     <row r="4" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="8"/>
       <c r="B4">
         <v>7</v>
       </c>
@@ -1056,7 +1036,7 @@
       <c r="J4" s="4">
         <v>0</v>
       </c>
-      <c r="L4" s="9"/>
+      <c r="L4" s="8"/>
       <c r="M4">
         <v>7</v>
       </c>
@@ -1115,7 +1095,7 @@
       </c>
       <c r="AI4" s="2">
         <f>$F10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="2">
         <f>$G10</f>
@@ -1359,7 +1339,7 @@
       </c>
     </row>
     <row r="5" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="8"/>
       <c r="B5">
         <v>6</v>
       </c>
@@ -1387,7 +1367,7 @@
       <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="L5" s="9"/>
+      <c r="L5" s="8"/>
       <c r="M5">
         <v>6</v>
       </c>
@@ -1437,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="AG5" s="2">
-        <f t="shared" ref="AF5:CP5" si="2">IF(AG4=1,AG3,0)</f>
+        <f t="shared" ref="AG5:CP5" si="2">IF(AG4=1,AG3,0)</f>
         <v>0</v>
       </c>
       <c r="AH5" s="2">
@@ -1446,7 +1426,7 @@
       </c>
       <c r="AI5" s="2">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="2">
         <f t="shared" si="2"/>
@@ -1690,7 +1670,7 @@
       </c>
     </row>
     <row r="6" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -1718,7 +1698,7 @@
       <c r="J6" s="4">
         <v>0</v>
       </c>
-      <c r="L6" s="9"/>
+      <c r="L6" s="8"/>
       <c r="M6">
         <v>5</v>
       </c>
@@ -1765,7 +1745,7 @@
       </c>
     </row>
     <row r="7" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="B7">
         <v>4</v>
       </c>
@@ -1793,7 +1773,7 @@
       <c r="J7" s="4">
         <v>0</v>
       </c>
-      <c r="L7" s="9"/>
+      <c r="L7" s="8"/>
       <c r="M7">
         <v>4</v>
       </c>
@@ -1840,7 +1820,7 @@
       </c>
     </row>
     <row r="8" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
       <c r="B8">
         <v>3</v>
       </c>
@@ -1868,7 +1848,7 @@
       <c r="J8" s="4">
         <v>0</v>
       </c>
-      <c r="L8" s="9"/>
+      <c r="L8" s="8"/>
       <c r="M8">
         <v>3</v>
       </c>
@@ -1915,7 +1895,7 @@
       </c>
     </row>
     <row r="9" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
       <c r="B9">
         <v>2</v>
       </c>
@@ -1943,7 +1923,7 @@
       <c r="J9" s="4">
         <v>0</v>
       </c>
-      <c r="L9" s="9"/>
+      <c r="L9" s="8"/>
       <c r="M9">
         <v>2</v>
       </c>
@@ -1990,7 +1970,7 @@
       </c>
     </row>
     <row r="10" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="B10">
         <v>1</v>
       </c>
@@ -2004,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -2018,7 +1998,7 @@
       <c r="J10" s="4">
         <v>0</v>
       </c>
-      <c r="L10" s="9"/>
+      <c r="L10" s="8"/>
       <c r="M10">
         <v>1</v>
       </c>
@@ -2056,7 +2036,7 @@
       </c>
       <c r="W10" t="str">
         <f>(J10&amp;I10&amp;H10&amp;G10&amp;F10&amp;E10&amp;D10&amp;C10)</f>
-        <v>00001000</v>
+        <v>00000000</v>
       </c>
       <c r="X10" s="1"/>
       <c r="AE10" s="2">
@@ -2117,20 +2097,20 @@
       <c r="U11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W11" s="8" t="str">
+      <c r="W11" s="9" t="str">
         <f>(W3&amp;W4&amp;W5&amp;W6&amp;W7&amp;W8&amp;W9&amp;W10)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000001000</v>
-      </c>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="8"/>
+        <v>0000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
       <c r="AE11" s="3">
         <f>SUM(AE2:AE10)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
@@ -2199,27 +2179,27 @@
     </row>
     <row r="12" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
       <c r="L12" s="7"/>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2230,10 +2210,10 @@
     <mergeCell ref="N12:U12"/>
   </mergeCells>
   <conditionalFormatting sqref="N3:U10">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Started work on movements logic.
</commit_message>
<xml_diff>
--- a/Gambit/Chess.xlsx
+++ b/Gambit/Chess.xlsx
@@ -455,7 +455,7 @@
   <dimension ref="A1:CQ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="X6" s="1"/>
       <c r="AE6" s="2">
-        <f>SUM(BD5:BK5)</f>
+        <f>SUM(BL5:BS5)</f>
         <v>0</v>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="X7" s="1"/>
       <c r="AE7" s="2">
-        <f>SUM(BL5:BS5)</f>
+        <f>SUM(BT5:CA5)</f>
         <v>0</v>
       </c>
     </row>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="X8" s="1"/>
       <c r="AE8" s="2">
-        <f>SUM(BT5:CA5)</f>
+        <f>SUM(CB5:CI5)</f>
         <v>0</v>
       </c>
     </row>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="X9" s="1"/>
       <c r="AE9" s="2">
-        <f>SUM(CB5:CI5)</f>
+        <f>SUM(CJ5:CQ5)</f>
         <v>0</v>
       </c>
     </row>
@@ -2039,8 +2039,8 @@
         <v>00000000</v>
       </c>
       <c r="X10" s="1"/>
-      <c r="AE10" s="2">
-        <f>SUM(CJ5:CQ5)</f>
+      <c r="AE10" s="3">
+        <f>SUM(AE2:AE9)</f>
         <v>0</v>
       </c>
     </row>
@@ -2108,10 +2108,6 @@
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="9"/>
-      <c r="AE11" s="3">
-        <f>SUM(AE2:AE10)</f>
-        <v>0</v>
-      </c>
       <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>

</xml_diff>